<commit_message>
add fs & txt change methods
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\da1_0\Programming\excel-replaceer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1CA747-60B4-4F0A-9C75-7E73C45C56C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB1B076-4755-495F-9E56-365BD3A738DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31170" yWindow="4455" windowWidth="17280" windowHeight="8970" xr2:uid="{68D0F4AB-BD86-48B5-B850-86DDB134C699}"/>
   </bookViews>
@@ -27,10 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>test.site</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>dummy</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -39,11 +35,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>test.site/test/</t>
+    <t>test02</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>test02</t>
+    <t>test01.html</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test02.html</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -411,7 +411,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H9:H10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -423,24 +423,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>